<commit_message>
TENSADRONE PACK, RaFi schematics
</commit_message>
<xml_diff>
--- a/ROD-MANIPULATOR/Project Outputs for RodManipulator_PRJ/BOM/Bill of Materials-BOM.xlsx
+++ b/ROD-MANIPULATOR/Project Outputs for RodManipulator_PRJ/BOM/Bill of Materials-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\UAV-CAN-MODULES\ROD-MANIPULATOR\Project Outputs for RodManipulator_PRJ\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33433206-35D1-4F09-BE6A-CC0CD80466CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{031AF59F-0B7D-40C6-BC10-5E7B296E6681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10125" xr2:uid="{05776390-B315-4E91-951E-E7F3357E41A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10125" xr2:uid="{9787EA68-82FE-4F12-A01E-AF6352405050}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-BOM" sheetId="1" r:id="rId1"/>
@@ -809,7 +809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9679482A-1BB7-49A5-B577-51CF7B7BB63E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192D1E35-4381-493F-81A5-2BBF9E76E15C}">
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>